<commit_message>
adds metadata to explain that NA values in redd data indicate 'not available'
</commit_message>
<xml_diff>
--- a/data-raw/metadata/steelhead-and-lamprey-redd-metadata.xlsx
+++ b/data-raw/metadata/steelhead-and-lamprey-redd-metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/stanislaus-steelhead/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445A4DA2-829F-2B4A-8580-49DA1358DB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB188104-B5F3-C14C-BF9D-DCA62796B526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,63 +196,12 @@
     <t>Longitude redd was sampled at</t>
   </si>
   <si>
-    <t>Species of redd</t>
-  </si>
-  <si>
     <t>Age of redd</t>
   </si>
   <si>
     <t>Estimated area of redd</t>
   </si>
   <si>
-    <t>Ambient depth of redd</t>
-  </si>
-  <si>
-    <t>Length of pot used to measure redd</t>
-  </si>
-  <si>
-    <t>Width of pot used to measure redd</t>
-  </si>
-  <si>
-    <t>Depth of pot used to measure redd</t>
-  </si>
-  <si>
-    <t>Tailspin length of redd</t>
-  </si>
-  <si>
-    <t>Tailspin width of redd</t>
-  </si>
-  <si>
-    <t>Estimated pot substrate</t>
-  </si>
-  <si>
-    <t>Estimated tailspin substrate</t>
-  </si>
-  <si>
-    <t>Estimated ambient substrate</t>
-  </si>
-  <si>
-    <t>Ambient velocity</t>
-  </si>
-  <si>
-    <t>Average velocity</t>
-  </si>
-  <si>
-    <t>Whether or not fish were present on the redd</t>
-  </si>
-  <si>
-    <t>Sex of fish number one</t>
-  </si>
-  <si>
-    <t>Estimated size of fish number one</t>
-  </si>
-  <si>
-    <t>Sex of fish number two</t>
-  </si>
-  <si>
-    <t>Estimated size of fish number two</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -304,13 +253,64 @@
     <t>est_area_m</t>
   </si>
   <si>
-    <t>Distance from the pot to the nearest submerged cover (log, bush, boulder)</t>
-  </si>
-  <si>
-    <t>Distance from the pot to the closest shore</t>
-  </si>
-  <si>
-    <t>Distance from the pot to the middle of the river in meters</t>
+    <t xml:space="preserve">Species associated with redd. </t>
+  </si>
+  <si>
+    <t>Ambient depth of redd. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Length of pot used to measure redd. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Width of pot used to measure redd. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Depth of pot used to measure redd. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Tailspin length of redd. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Tailspin width of redd. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Estimated pot substrate. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Estimated tailspin substrate. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Estimated ambient substrate. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Ambient velocity. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Average velocity. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Distance from the pot to the nearest submerged cover (log, bush, boulder). NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Distance from the pot to the closest shore. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Distance from the pot to the middle of the river in meters. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Whether or not fish were present on the redd. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Sex of fish number one. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Estimated size of fish number one. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Sex of fish number two. NA values indicate "not available"</t>
+  </si>
+  <si>
+    <t>Estimated size of fish number two. NA values indicate "not available"</t>
   </si>
 </sst>
 </file>
@@ -765,7 +765,7 @@
   <dimension ref="A1:AMG33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,27 +835,27 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="5"/>
       <c r="J2" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="7" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -866,13 +866,13 @@
         <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -891,13 +891,13 @@
         <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -916,13 +916,13 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -941,13 +941,13 @@
         <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -966,13 +966,13 @@
         <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -991,13 +991,13 @@
         <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1016,13 +1016,13 @@
         <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1041,13 +1041,13 @@
         <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="6"/>
@@ -1063,16 +1063,16 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1088,25 +1088,25 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="3"/>
@@ -1120,19 +1120,19 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1148,25 +1148,25 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="3"/>
@@ -1183,16 +1183,16 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1208,16 +1208,16 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1233,16 +1233,16 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
         <v>62</v>
-      </c>
-      <c r="C17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" t="s">
-        <v>79</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1258,25 +1258,25 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="3"/>
@@ -1293,25 +1293,25 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="3"/>
@@ -1328,25 +1328,25 @@
         <v>33</v>
       </c>
       <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" t="s">
-        <v>82</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="3"/>
@@ -1363,25 +1363,25 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="3"/>
@@ -1398,25 +1398,25 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="H22" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="3"/>
@@ -1433,25 +1433,25 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="H23" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="3"/>
@@ -1468,25 +1468,25 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="3"/>
@@ -1503,25 +1503,25 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="3"/>
@@ -1538,25 +1538,25 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="3"/>
@@ -1573,25 +1573,25 @@
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="3"/>
@@ -1608,16 +1608,16 @@
         <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1633,16 +1633,16 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1658,16 +1658,16 @@
         <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1683,16 +1683,16 @@
         <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1708,16 +1708,16 @@
         <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -1733,16 +1733,16 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>

</xml_diff>